<commit_message>
Actualizar la función 'libro_diario' para insertar múltiples registros en el archivo Excel desde el formulario, mejorando la gestión de datos y la estructura del archivo.
</commit_message>
<xml_diff>
--- a/LDE.xlsx
+++ b/LDE.xlsx
@@ -931,7 +931,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K183"/>
+  <dimension ref="A1:K185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -961,11 +961,11 @@
       <c r="D1" s="3" t="n"/>
       <c r="E1" s="3" t="n"/>
       <c r="F1" s="4">
-        <f>SUM(F3:F15)</f>
+        <f>SUM(F3:F24)</f>
         <v/>
       </c>
       <c r="G1" s="4">
-        <f>SUM(G3:G15)</f>
+        <f>SUM(G3:G24)</f>
         <v/>
       </c>
       <c r="H1" s="5">
@@ -1463,117 +1463,315 @@
       <c r="K15" s="3" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="8" t="n"/>
-      <c r="B16" s="10" t="n"/>
-      <c r="C16" s="10" t="n"/>
-      <c r="D16" s="11" t="n"/>
-      <c r="E16" s="13" t="n"/>
-      <c r="F16" s="12" t="n"/>
-      <c r="G16" s="12" t="n"/>
+      <c r="A16" s="8" t="inlineStr">
+        <is>
+          <t>2001-09-18</t>
+        </is>
+      </c>
+      <c r="B16" s="10" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="C16" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11" t="inlineStr">
+        <is>
+          <t>11111- CAJA</t>
+        </is>
+      </c>
+      <c r="E16" s="13" t="inlineStr">
+        <is>
+          <t>Probando</t>
+        </is>
+      </c>
+      <c r="F16" s="12" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G16" s="12" t="n">
+        <v>10000</v>
+      </c>
       <c r="H16" s="3" t="n"/>
       <c r="I16" s="3" t="n"/>
       <c r="J16" s="3" t="n"/>
       <c r="K16" s="3" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="8" t="n"/>
-      <c r="B17" s="10" t="n"/>
-      <c r="C17" s="10" t="n"/>
-      <c r="D17" s="11" t="n"/>
-      <c r="E17" s="13" t="n"/>
-      <c r="F17" s="12" t="n"/>
-      <c r="G17" s="12" t="n"/>
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>2001-09-18</t>
+        </is>
+      </c>
+      <c r="B17" s="10" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="C17" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" s="11" t="inlineStr">
+        <is>
+          <t>11111- CAJA</t>
+        </is>
+      </c>
+      <c r="E17" s="13" t="inlineStr">
+        <is>
+          <t>testing</t>
+        </is>
+      </c>
+      <c r="F17" s="12" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G17" s="12" t="n">
+        <v>10000</v>
+      </c>
       <c r="H17" s="3" t="n"/>
       <c r="I17" s="3" t="n"/>
       <c r="J17" s="3" t="n"/>
       <c r="K17" s="3" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="8" t="n"/>
-      <c r="B18" s="10" t="n"/>
-      <c r="C18" s="10" t="n"/>
-      <c r="D18" s="11" t="n"/>
-      <c r="E18" s="11" t="n"/>
-      <c r="F18" s="12" t="n"/>
-      <c r="G18" s="12" t="n"/>
+      <c r="A18" s="8" t="inlineStr">
+        <is>
+          <t>16-06-2004</t>
+        </is>
+      </c>
+      <c r="B18" s="10" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C18" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" s="11" t="inlineStr">
+        <is>
+          <t>11111- CAJA</t>
+        </is>
+      </c>
+      <c r="E18" s="11" t="inlineStr">
+        <is>
+          <t>Ultima</t>
+        </is>
+      </c>
+      <c r="F18" s="12" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G18" s="12" t="n">
+        <v>10000</v>
+      </c>
       <c r="H18" s="3" t="n"/>
       <c r="I18" s="3" t="n"/>
       <c r="J18" s="3" t="n"/>
       <c r="K18" s="3" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="8" t="n"/>
-      <c r="B19" s="10" t="n"/>
-      <c r="C19" s="10" t="n"/>
-      <c r="D19" s="11" t="n"/>
-      <c r="E19" s="11" t="n"/>
-      <c r="F19" s="12" t="n"/>
-      <c r="G19" s="12" t="n"/>
+      <c r="A19" s="8" t="inlineStr">
+        <is>
+          <t>18-09-2001</t>
+        </is>
+      </c>
+      <c r="B19" s="10" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C19" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" s="11" t="inlineStr">
+        <is>
+          <t>11111- CAJA</t>
+        </is>
+      </c>
+      <c r="E19" s="11" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="F19" s="12" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G19" s="12" t="n">
+        <v>0</v>
+      </c>
       <c r="H19" s="3" t="n"/>
       <c r="I19" s="3" t="n"/>
       <c r="J19" s="3" t="n"/>
       <c r="K19" s="3" t="n"/>
     </row>
     <row r="20" ht="18.75" customHeight="1" s="89">
-      <c r="A20" s="8" t="n"/>
-      <c r="B20" s="10" t="n"/>
-      <c r="C20" s="10" t="n"/>
-      <c r="D20" s="11" t="n"/>
-      <c r="E20" s="11" t="n"/>
-      <c r="F20" s="12" t="n"/>
-      <c r="G20" s="12" t="n"/>
+      <c r="A20" s="8" t="inlineStr">
+        <is>
+          <t>18-09-2002</t>
+        </is>
+      </c>
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C20" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" s="11" t="inlineStr">
+        <is>
+          <t>12111- CLIENTES</t>
+        </is>
+      </c>
+      <c r="E20" s="11" t="inlineStr">
+        <is>
+          <t>Metro</t>
+        </is>
+      </c>
+      <c r="F20" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12" t="n">
+        <v>2000</v>
+      </c>
       <c r="H20" s="3" t="n"/>
       <c r="I20" s="3" t="n"/>
       <c r="J20" s="3" t="n"/>
       <c r="K20" s="3" t="n"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="89">
-      <c r="A21" s="8" t="n"/>
-      <c r="B21" s="10" t="n"/>
-      <c r="C21" s="10" t="n"/>
-      <c r="D21" s="11" t="n"/>
-      <c r="E21" s="11" t="n"/>
-      <c r="F21" s="12" t="n"/>
-      <c r="G21" s="12" t="n"/>
+      <c r="A21" s="8" t="inlineStr">
+        <is>
+          <t>02-12-2004</t>
+        </is>
+      </c>
+      <c r="B21" s="10" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C21" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" s="11" t="inlineStr">
+        <is>
+          <t>31313- GASTOS BANCARIOS</t>
+        </is>
+      </c>
+      <c r="E21" s="11" t="inlineStr">
+        <is>
+          <t>gastos</t>
+        </is>
+      </c>
+      <c r="F21" s="12" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G21" s="12" t="n">
+        <v>0</v>
+      </c>
       <c r="H21" s="3" t="n"/>
       <c r="I21" s="3" t="n"/>
       <c r="J21" s="3" t="n"/>
       <c r="K21" s="3" t="n"/>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="89">
-      <c r="A22" s="8" t="n"/>
-      <c r="B22" s="10" t="n"/>
-      <c r="C22" s="10" t="n"/>
-      <c r="D22" s="11" t="n"/>
-      <c r="E22" s="11" t="n"/>
-      <c r="F22" s="12" t="n"/>
-      <c r="G22" s="12" t="n"/>
+      <c r="A22" s="8" t="inlineStr">
+        <is>
+          <t>02-12-2004</t>
+        </is>
+      </c>
+      <c r="B22" s="10" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C22" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D22" s="11" t="inlineStr">
+        <is>
+          <t>11112- BANCO</t>
+        </is>
+      </c>
+      <c r="E22" s="11" t="inlineStr">
+        <is>
+          <t>gastos</t>
+        </is>
+      </c>
+      <c r="F22" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="12" t="n">
+        <v>10000</v>
+      </c>
       <c r="H22" s="3" t="n"/>
       <c r="I22" s="3" t="n"/>
       <c r="J22" s="3" t="n"/>
       <c r="K22" s="3" t="n"/>
     </row>
     <row r="23" ht="15.75" customHeight="1" s="89">
-      <c r="A23" s="14" t="n"/>
-      <c r="B23" s="9" t="n"/>
-      <c r="C23" s="10" t="n"/>
-      <c r="D23" s="11" t="n"/>
-      <c r="E23" s="11" t="n"/>
-      <c r="F23" s="12" t="n"/>
-      <c r="G23" s="12" t="n"/>
+      <c r="A23" s="14" t="inlineStr">
+        <is>
+          <t>02-12-2004</t>
+        </is>
+      </c>
+      <c r="B23" s="9" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C23" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D23" s="11" t="inlineStr">
+        <is>
+          <t>31313- GASTOS BANCARIOS</t>
+        </is>
+      </c>
+      <c r="E23" s="11" t="inlineStr">
+        <is>
+          <t>gastos</t>
+        </is>
+      </c>
+      <c r="F23" s="12" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G23" s="12" t="n">
+        <v>0</v>
+      </c>
       <c r="H23" s="3" t="n"/>
       <c r="I23" s="3" t="n"/>
       <c r="J23" s="3" t="n"/>
       <c r="K23" s="3" t="n"/>
     </row>
     <row r="24" ht="15.75" customHeight="1" s="89">
-      <c r="A24" s="14" t="n"/>
-      <c r="B24" s="9" t="n"/>
-      <c r="C24" s="10" t="n"/>
-      <c r="D24" s="11" t="n"/>
-      <c r="E24" s="11" t="n"/>
-      <c r="F24" s="12" t="n"/>
-      <c r="G24" s="12" t="n"/>
+      <c r="A24" s="14" t="inlineStr">
+        <is>
+          <t>02-12-2004</t>
+        </is>
+      </c>
+      <c r="B24" s="9" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C24" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D24" s="11" t="inlineStr">
+        <is>
+          <t>11112- BANCO</t>
+        </is>
+      </c>
+      <c r="E24" s="11" t="inlineStr">
+        <is>
+          <t>gastos</t>
+        </is>
+      </c>
+      <c r="F24" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="12" t="n">
+        <v>10000</v>
+      </c>
       <c r="H24" s="3" t="n"/>
       <c r="I24" s="3" t="n"/>
       <c r="J24" s="3" t="n"/>
@@ -3645,6 +3843,68 @@
       <c r="I183" s="3" t="n"/>
       <c r="J183" s="3" t="n"/>
       <c r="K183" s="3" t="n"/>
+    </row>
+    <row r="184">
+      <c r="A184" s="0" t="inlineStr">
+        <is>
+          <t>2001-09-18</t>
+        </is>
+      </c>
+      <c r="B184" s="0" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="C184" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="D184" s="0" t="inlineStr">
+        <is>
+          <t>11111- CAJA</t>
+        </is>
+      </c>
+      <c r="E184" s="0" t="inlineStr">
+        <is>
+          <t>Probando</t>
+        </is>
+      </c>
+      <c r="F184" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G184" s="0" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="0" t="inlineStr">
+        <is>
+          <t>2001-01-01</t>
+        </is>
+      </c>
+      <c r="B185" s="0" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="C185" s="0" t="n">
+        <v>184</v>
+      </c>
+      <c r="D185" s="0" t="inlineStr">
+        <is>
+          <t>12121- IVA CREDITO</t>
+        </is>
+      </c>
+      <c r="E185" s="0" t="inlineStr">
+        <is>
+          <t>No se</t>
+        </is>
+      </c>
+      <c r="F185" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G185" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="$A$2:$G$181"/>

</xml_diff>